<commit_message>
edits to ODD writing schema rules: few working as of today's meeting
</commit_message>
<xml_diff>
--- a/ODD_Schema/SCHEMArules_NOTES.xlsx
+++ b/ODD_Schema/SCHEMArules_NOTES.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rebecca Parker\Documents\GitHub\Thomas-Bartram-Digital-Archives\ODD_Schema\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="2140" windowWidth="13520" windowHeight="12900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="2640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
   <si>
     <t>BARTRAM SCHEMA NOTES</t>
   </si>
@@ -112,12 +117,21 @@
   </si>
   <si>
     <t>illegible, strikethrough</t>
+  </si>
+  <si>
+    <t>always have a page with @facs may or maynot have @subtype</t>
+  </si>
+  <si>
+    <t>always have at least one div group in a page</t>
+  </si>
+  <si>
+    <t>list must have a head if parent div group doesn't</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -333,6 +347,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -658,24 +680,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -686,7 +708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -696,16 +718,22 @@
       <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1">
+      <c r="D4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -716,7 +744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -724,7 +752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -734,8 +762,11 @@
       <c r="C10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -743,7 +774,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -754,7 +785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -762,7 +793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -770,7 +801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -778,7 +809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -786,7 +817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -794,7 +825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -802,7 +833,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -813,7 +844,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -821,7 +852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -829,7 +860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -837,7 +868,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -845,7 +876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>13</v>
       </c>
@@ -853,7 +884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -861,7 +892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -869,7 +900,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -877,7 +908,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -885,7 +916,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -896,7 +927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -907,7 +938,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -918,7 +949,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -929,7 +960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>25</v>
       </c>

</xml_diff>